<commit_message>
modificacion archivos de excel
</commit_message>
<xml_diff>
--- a/app/assets/formatsXlsx/Carga_Fabril.xlsx
+++ b/app/assets/formatsXlsx/Carga_Fabril.xlsx
@@ -1,16 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\desarrollo\apps\htdocs\tezlikv2\app\assets\formatsXlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ED9A33-54E8-44CD-90EA-63207E4C7A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="19920" windowHeight="8520"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sergio Eduardo Velandia Obando</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CC3B3599-2128-4916-B79D-24D9B305AA95}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Teenus: No modifique los encabezados. Son necesarios al momento de importar los datos</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -38,15 +80,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
+      <name val="Roboto"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -136,28 +178,26 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -172,16 +212,14 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial Unicode MS"/>
+        <name val="Roboto"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -196,14 +234,16 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial Unicode MS"/>
+        <name val="Roboto"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -218,13 +258,13 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial Unicode MS"/>
+        <name val="Roboto"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -263,12 +303,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial Unicode MS"/>
+        <name val="Roboto"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <right style="thin">
           <color indexed="64"/>
@@ -290,12 +330,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="16"/>
+        <sz val="12"/>
         <color theme="1"/>
-        <name val="Arial Unicode MS"/>
+        <name val="Roboto"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -309,15 +349,23 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="2" name="maquina" dataDxfId="2"/>
-    <tableColumn id="1" name="descripcion" dataDxfId="0"/>
-    <tableColumn id="3" name="costo" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="maquina" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="descripcion" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="costo" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -366,7 +414,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,9 +446,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,6 +498,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -607,76 +691,78 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="20.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:3" ht="20.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:3" ht="20.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:3" ht="20.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>